<commit_message>
convyer code + arm base movment test code
</commit_message>
<xml_diff>
--- a/Connection Pins.xlsx
+++ b/Connection Pins.xlsx
@@ -1,25 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\My Files\Hardware GP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2725D49B-8C3A-44EB-A41C-AA859450C56E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104E4FCB-57B3-4800-89D3-848DCAAAE83B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6A5D1260-6494-4CBC-B724-ECEB29E07873}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -34,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Arduino PIN</t>
   </si>
@@ -45,6 +42,9 @@
     <t>Element PIN</t>
   </si>
   <si>
+    <t>Driver-Convire (1)</t>
+  </si>
+  <si>
     <t>dir</t>
   </si>
   <si>
@@ -54,25 +54,58 @@
     <t>En</t>
   </si>
   <si>
-    <t>Driver-Convire (1)</t>
-  </si>
-  <si>
     <t>Driver Trail-Convire (2)</t>
   </si>
   <si>
-    <t>ldr</t>
+    <t>ldr1</t>
+  </si>
+  <si>
+    <t>ldr2</t>
+  </si>
+  <si>
+    <t>limit switch</t>
+  </si>
+  <si>
+    <t>trail</t>
+  </si>
+  <si>
+    <t>convire</t>
+  </si>
+  <si>
+    <t>s1</t>
+  </si>
+  <si>
+    <t>s2</t>
+  </si>
+  <si>
+    <t>s3</t>
+  </si>
+  <si>
+    <t>s4</t>
+  </si>
+  <si>
+    <t>s5</t>
+  </si>
+  <si>
+    <t>s6</t>
+  </si>
+  <si>
+    <t>PIN</t>
+  </si>
+  <si>
+    <t>Servo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -85,18 +118,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -104,16 +137,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -175,7 +227,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -208,26 +260,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -260,23 +295,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -419,79 +437,122 @@
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EA57D29-01A9-4886-BDDB-C809003A17B4}">
-  <dimension ref="A1:C10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="12.21875" customWidth="1"/>
     <col min="2" max="2" width="22.77734375" customWidth="1"/>
     <col min="3" max="3" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:20">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="N1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
       <c r="A2" s="3">
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="5">
+        <v>11</v>
+      </c>
+      <c r="P2" s="5">
+        <v>12</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>13</v>
+      </c>
+      <c r="R2" s="5">
+        <v>50</v>
+      </c>
+      <c r="S2" s="5">
+        <v>51</v>
+      </c>
+      <c r="T2" s="5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
       <c r="A3" s="3">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
       <c r="A4" s="3">
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:20">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="K5" s="4">
+        <v>2</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -499,10 +560,14 @@
         <v>7</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" spans="1:20">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -510,10 +575,14 @@
         <v>7</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K7" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8" spans="1:20">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -521,16 +590,72 @@
         <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="K9" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="L9" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
       <c r="A10" s="3">
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="K10" s="4">
+        <v>6</v>
+      </c>
+      <c r="L10" s="4"/>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K11" s="4">
+        <v>7</v>
+      </c>
+      <c r="L11" s="4"/>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>